<commit_message>
Complete the figures and results interpretation.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuhe/Desktop/meta analysis/BPA_cancer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7903F2F-CC21-C44D-B73A-50BDFA2213FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18707F26-1241-864A-8DD4-F10D836E1910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" activeTab="1" xr2:uid="{257D24D0-6FF3-2444-9E9F-0EFE0C722110}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{257D24D0-6FF3-2444-9E9F-0EFE0C722110}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_analysis" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="43">
   <si>
     <t>Random effects model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -196,6 +196,10 @@
   </si>
   <si>
     <t>1 (SE = 2.0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>General model</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -629,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83076C81-D8E1-2A49-BBE0-33D4E96C216D}">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -640,7 +644,7 @@
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -649,6 +653,7 @@
     <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -747,9 +752,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="33" customHeight="1">
+    <row r="3" spans="1:20" ht="17">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -762,72 +767,72 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="1">
-        <v>1.3311999999999999</v>
+        <v>1.4512</v>
       </c>
       <c r="C4" s="1">
-        <v>1.0775999999999999</v>
+        <v>1.1583000000000001</v>
       </c>
       <c r="D4" s="1">
-        <v>1.6446000000000001</v>
+        <v>1.8183</v>
       </c>
       <c r="E4" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="F4" s="1">
-        <v>0.14729999999999999</v>
+        <v>0.18709999999999999</v>
       </c>
       <c r="G4" s="1">
-        <v>6.2199999999999998E-2</v>
+        <v>0.11020000000000001</v>
       </c>
       <c r="H4" s="1">
-        <v>0.53779999999999994</v>
+        <v>1.1082000000000001</v>
       </c>
       <c r="I4" s="1">
-        <v>0.38379999999999997</v>
+        <v>0.4325</v>
       </c>
       <c r="J4" s="1">
-        <v>0.2495</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="K4" s="1">
-        <v>0.73340000000000005</v>
+        <v>1.0527</v>
       </c>
       <c r="L4" s="4">
-        <v>0.77800000000000002</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0.65800000000000003</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0.85599999999999998</v>
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0.84599999999999997</v>
       </c>
       <c r="O4" s="1">
-        <v>2.12</v>
-      </c>
-      <c r="P4" s="1">
-        <v>1.71</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>2.63</v>
-      </c>
-      <c r="R4" s="1">
-        <v>81.08</v>
-      </c>
-      <c r="S4" s="1">
-        <v>18</v>
+        <v>2.09</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1.72</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="R4" s="2">
+        <v>96.53</v>
+      </c>
+      <c r="S4" s="2">
+        <v>22</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>20</v>
@@ -838,66 +843,66 @@
         <v>19</v>
       </c>
       <c r="B5" s="1">
-        <v>1.2327999999999999</v>
+        <v>1.3349</v>
       </c>
       <c r="C5" s="1">
-        <v>1.0255000000000001</v>
+        <v>1.0889</v>
       </c>
       <c r="D5" s="1">
-        <v>1.4822</v>
+        <v>1.6364000000000001</v>
       </c>
       <c r="E5" s="1">
-        <v>2.5899999999999999E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="F5" s="1">
-        <v>0.1007</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="G5" s="1">
-        <v>4.2099999999999999E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="H5" s="1">
-        <v>0.47760000000000002</v>
+        <v>1.1132</v>
       </c>
       <c r="I5" s="1">
-        <v>0.31730000000000003</v>
+        <v>0.37569999999999998</v>
       </c>
       <c r="J5" s="1">
-        <v>0.20530000000000001</v>
+        <v>0.30719999999999997</v>
       </c>
       <c r="K5" s="1">
-        <v>0.69110000000000005</v>
+        <v>1.0550999999999999</v>
       </c>
       <c r="L5" s="4">
         <v>0.748</v>
       </c>
-      <c r="M5" s="4">
-        <v>0.60499999999999998</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0.83899999999999997</v>
+      <c r="M5" s="6">
+        <v>0.621</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0.83199999999999996</v>
       </c>
       <c r="O5" s="1">
         <v>1.99</v>
       </c>
-      <c r="P5" s="1">
-        <v>1.59</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="R5" s="1">
-        <v>71.290000000000006</v>
-      </c>
-      <c r="S5" s="1">
-        <v>18</v>
+      <c r="P5" s="2">
+        <v>1.63</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>2.44</v>
+      </c>
+      <c r="R5" s="2">
+        <v>87.21</v>
+      </c>
+      <c r="S5" s="2">
+        <v>22</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="5" t="s">
-        <v>25</v>
+    <row r="6" spans="1:20" ht="33" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -920,156 +925,156 @@
       <c r="T6" s="1"/>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.3311999999999999</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.0775999999999999</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.6446000000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.14729999999999999</v>
+      </c>
+      <c r="G7" s="1">
+        <v>6.2199999999999998E-2</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.53779999999999994</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.38379999999999997</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.2495</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.73340000000000005</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="O7" s="1">
+        <v>2.12</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1.71</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>2.63</v>
+      </c>
+      <c r="R7" s="1">
+        <v>81.08</v>
+      </c>
+      <c r="S7" s="1">
+        <v>18</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1.5121</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1.1851</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.9294</v>
-      </c>
-      <c r="E8" s="2">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="F8" s="2">
-        <v>9.7000000000000003E-2</v>
-      </c>
-      <c r="G8" s="2">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1.1774</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0.3115</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.18970000000000001</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1.0851</v>
-      </c>
-      <c r="L8" s="6">
-        <v>0.753</v>
-      </c>
-      <c r="M8" s="6">
-        <v>0.52300000000000002</v>
-      </c>
-      <c r="N8" s="6">
-        <v>0.872</v>
-      </c>
-      <c r="O8" s="2">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="P8" s="2">
-        <v>1.45</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>2.79</v>
-      </c>
-      <c r="R8" s="2">
-        <v>32.35</v>
-      </c>
-      <c r="S8" s="2">
-        <v>8</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.2327999999999999</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.0255000000000001</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.4822</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.1007</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4.2099999999999999E-2</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.47760000000000002</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.20530000000000001</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.69110000000000005</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0.748</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="O8" s="1">
+        <v>1.99</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1.59</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="R8" s="1">
+        <v>71.290000000000006</v>
+      </c>
+      <c r="S8" s="1">
+        <v>18</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1.4006000000000001</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1.1574</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.6949000000000001</v>
-      </c>
-      <c r="E9" s="2">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="F9" s="2">
-        <v>4.9200000000000001E-2</v>
-      </c>
-      <c r="G9" s="2">
-        <v>2.7300000000000001E-2</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1.1476999999999999</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0.2218</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0.16520000000000001</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1.0712999999999999</v>
-      </c>
-      <c r="L9" s="6">
-        <v>0.71599999999999997</v>
-      </c>
-      <c r="M9" s="6">
-        <v>0.441</v>
-      </c>
-      <c r="N9" s="6">
-        <v>0.85599999999999998</v>
-      </c>
-      <c r="O9" s="2">
-        <v>1.88</v>
-      </c>
-      <c r="P9" s="2">
-        <v>1.34</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>2.64</v>
-      </c>
-      <c r="R9" s="2">
-        <v>28.22</v>
-      </c>
-      <c r="S9" s="2">
-        <v>8</v>
-      </c>
-      <c r="T9" s="1">
-        <v>4.0000000000000002E-4</v>
-      </c>
+      <c r="A9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1092,132 +1097,132 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="2" t="s">
-        <v>16</v>
+      <c r="A11" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B11" s="2">
-        <v>1.1416999999999999</v>
+        <v>1.5121</v>
       </c>
       <c r="C11" s="2">
-        <v>0.84460000000000002</v>
+        <v>1.1851</v>
       </c>
       <c r="D11" s="2">
-        <v>1.5432999999999999</v>
+        <v>1.9294</v>
       </c>
       <c r="E11" s="2">
-        <v>0.38890000000000002</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="F11" s="2">
-        <v>0.13339999999999999</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="G11" s="2">
-        <v>1.5900000000000001E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="H11" s="2">
-        <v>0.76259999999999994</v>
+        <v>1.1774</v>
       </c>
       <c r="I11" s="2">
-        <v>0.36530000000000001</v>
+        <v>0.3115</v>
       </c>
       <c r="J11" s="2">
-        <v>0.12590000000000001</v>
+        <v>0.18970000000000001</v>
       </c>
       <c r="K11" s="2">
-        <v>0.87329999999999997</v>
-      </c>
-      <c r="L11" s="4">
-        <v>0.61099999999999999</v>
+        <v>1.0851</v>
+      </c>
+      <c r="L11" s="6">
+        <v>0.753</v>
       </c>
       <c r="M11" s="6">
-        <v>0.22500000000000001</v>
+        <v>0.52300000000000002</v>
       </c>
       <c r="N11" s="6">
-        <v>0.80500000000000005</v>
+        <v>0.872</v>
       </c>
       <c r="O11" s="2">
-        <v>1.6</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="P11" s="2">
-        <v>1.1399999999999999</v>
+        <v>1.45</v>
       </c>
       <c r="Q11" s="2">
-        <v>2.27</v>
+        <v>2.79</v>
       </c>
       <c r="R11" s="2">
-        <v>23.16</v>
+        <v>32.35</v>
       </c>
       <c r="S11" s="2">
-        <v>9</v>
-      </c>
-      <c r="T11" s="2">
-        <v>5.7999999999999996E-3</v>
+        <v>8</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="2" t="s">
-        <v>18</v>
+      <c r="A12" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B12" s="2">
-        <v>1.0134000000000001</v>
+        <v>1.4006000000000001</v>
       </c>
       <c r="C12" s="2">
-        <v>0.84089999999999998</v>
+        <v>1.1574</v>
       </c>
       <c r="D12" s="2">
-        <v>1.2212000000000001</v>
+        <v>1.6949000000000001</v>
       </c>
       <c r="E12" s="2">
-        <v>0.8891</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="F12" s="2">
-        <v>2.7199999999999998E-2</v>
+        <v>4.9200000000000001E-2</v>
       </c>
       <c r="G12" s="2">
-        <v>0</v>
+        <v>2.7300000000000001E-2</v>
       </c>
       <c r="H12" s="2">
-        <v>0.62080000000000002</v>
+        <v>1.1476999999999999</v>
       </c>
       <c r="I12" s="2">
-        <v>0.16489999999999999</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
+        <v>0.2218</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.16520000000000001</v>
       </c>
       <c r="K12" s="2">
-        <v>0.78790000000000004</v>
+        <v>1.0712999999999999</v>
       </c>
       <c r="L12" s="6">
-        <v>0.436</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="M12" s="6">
-        <v>0</v>
+        <v>0.441</v>
       </c>
       <c r="N12" s="6">
-        <v>0.72899999999999998</v>
+        <v>0.85599999999999998</v>
       </c>
       <c r="O12" s="2">
-        <v>1.33</v>
+        <v>1.88</v>
       </c>
       <c r="P12" s="2">
-        <v>1</v>
+        <v>1.34</v>
       </c>
       <c r="Q12" s="2">
-        <v>1.92</v>
+        <v>2.64</v>
       </c>
       <c r="R12" s="2">
-        <v>15.94</v>
+        <v>28.22</v>
       </c>
       <c r="S12" s="2">
-        <v>9</v>
-      </c>
-      <c r="T12" s="2">
-        <v>6.8000000000000005E-2</v>
+        <v>8</v>
+      </c>
+      <c r="T12" s="1">
+        <v>4.0000000000000002E-4</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1240,218 +1245,237 @@
       <c r="T13" s="1"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.1416999999999999</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.84460000000000002</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.5432999999999999</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.38890000000000002</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.13339999999999999</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.76259999999999994</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.36530000000000001</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.12590000000000001</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.87329999999999997</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="M14" s="6">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="O14" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>2.27</v>
+      </c>
+      <c r="R14" s="2">
+        <v>23.16</v>
+      </c>
+      <c r="S14" s="2">
+        <v>9</v>
+      </c>
+      <c r="T14" s="2">
+        <v>5.7999999999999996E-3</v>
+      </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2">
-        <v>1.3977999999999999</v>
+        <v>1.0134000000000001</v>
       </c>
       <c r="C15" s="2">
-        <v>1.1185</v>
+        <v>0.84089999999999998</v>
       </c>
       <c r="D15" s="2">
-        <v>1.7466999999999999</v>
+        <v>1.2212000000000001</v>
       </c>
       <c r="E15" s="2">
-        <v>3.2000000000000002E-3</v>
+        <v>0.8891</v>
       </c>
       <c r="F15" s="2">
-        <v>0.13750000000000001</v>
+        <v>2.7199999999999998E-2</v>
       </c>
       <c r="G15" s="2">
-        <v>6.2E-2</v>
+        <v>0</v>
       </c>
       <c r="H15" s="2">
-        <v>0.66159999999999997</v>
+        <v>0.62080000000000002</v>
       </c>
       <c r="I15" s="2">
-        <v>0.37069999999999997</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0.249</v>
+        <v>0.16489999999999999</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
       </c>
       <c r="K15" s="2">
-        <v>0.81340000000000001</v>
+        <v>0.78790000000000004</v>
       </c>
       <c r="L15" s="6">
-        <v>0.81899999999999995</v>
+        <v>0.436</v>
       </c>
       <c r="M15" s="6">
-        <v>0.70699999999999996</v>
+        <v>0</v>
       </c>
       <c r="N15" s="6">
-        <v>0.88800000000000001</v>
+        <v>0.72899999999999998</v>
       </c>
       <c r="O15" s="2">
-        <v>2.35</v>
+        <v>1.33</v>
       </c>
       <c r="P15" s="2">
-        <v>1.85</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="2">
-        <v>2.99</v>
+        <v>1.92</v>
       </c>
       <c r="R15" s="2">
-        <v>71.69</v>
+        <v>15.94</v>
       </c>
       <c r="S15" s="2">
-        <v>13</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="T15" s="2">
+        <v>6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1.2757000000000001</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1.0528</v>
-      </c>
-      <c r="D16" s="2">
-        <v>1.5458000000000001</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="F16" s="2">
-        <v>9.3200000000000005E-2</v>
-      </c>
-      <c r="G16" s="2">
-        <v>4.3099999999999999E-2</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0.5927</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0.30530000000000002</v>
-      </c>
-      <c r="J16" s="1">
-        <v>0.20760000000000001</v>
-      </c>
-      <c r="K16" s="2">
-        <v>0.76990000000000003</v>
-      </c>
-      <c r="L16" s="4">
-        <v>0.79200000000000004</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0.65700000000000003</v>
-      </c>
-      <c r="N16" s="4">
-        <v>0.873</v>
-      </c>
-      <c r="O16" s="2">
-        <v>2.19</v>
-      </c>
-      <c r="P16" s="2">
-        <v>1.71</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>2.81</v>
-      </c>
-      <c r="R16" s="2">
-        <v>62.43</v>
-      </c>
-      <c r="S16" s="2">
-        <v>13</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="A16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2">
-        <v>0.9869</v>
+        <v>1.3977999999999999</v>
       </c>
       <c r="C18" s="2">
-        <v>0.58760000000000001</v>
+        <v>1.1185</v>
       </c>
       <c r="D18" s="2">
-        <v>1.6574</v>
+        <v>1.7466999999999999</v>
       </c>
       <c r="E18" s="2">
-        <v>0.96009999999999995</v>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="F18" s="2">
-        <v>0.1152</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="G18" s="2">
-        <v>0</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H18" s="2">
-        <v>2.9306000000000001</v>
+        <v>0.66159999999999997</v>
       </c>
       <c r="I18" s="2">
-        <v>0.33939999999999998</v>
+        <v>0.37069999999999997</v>
       </c>
       <c r="J18" s="2">
-        <v>0</v>
+        <v>0.249</v>
       </c>
       <c r="K18" s="2">
-        <v>1.7119</v>
+        <v>0.81340000000000001</v>
       </c>
       <c r="L18" s="6">
-        <v>0.317</v>
+        <v>0.81899999999999995</v>
       </c>
       <c r="M18" s="6">
-        <v>0</v>
+        <v>0.70699999999999996</v>
       </c>
       <c r="N18" s="6">
-        <v>0.73899999999999999</v>
+        <v>0.88800000000000001</v>
       </c>
       <c r="O18" s="2">
-        <v>1.21</v>
+        <v>2.35</v>
       </c>
       <c r="P18" s="2">
-        <v>1</v>
+        <v>1.85</v>
       </c>
       <c r="Q18" s="2">
-        <v>1.96</v>
+        <v>2.99</v>
       </c>
       <c r="R18" s="2">
-        <v>5.86</v>
+        <v>71.69</v>
       </c>
       <c r="S18" s="2">
-        <v>4</v>
-      </c>
-      <c r="T18" s="2">
-        <v>0.2102</v>
+        <v>13</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -1459,281 +1483,262 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
+        <v>1.2757000000000001</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.0528</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1.5458000000000001</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F19" s="2">
+        <v>9.3200000000000005E-2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.5927</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.30530000000000002</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.20760000000000001</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.76990000000000003</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="M19" s="4">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="N19" s="4">
+        <v>0.873</v>
+      </c>
+      <c r="O19" s="2">
+        <v>2.19</v>
+      </c>
+      <c r="P19" s="2">
+        <v>1.71</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>2.81</v>
+      </c>
+      <c r="R19" s="2">
+        <v>62.43</v>
+      </c>
+      <c r="S19" s="2">
+        <v>13</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2">
         <v>0.9869</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C21" s="2">
         <v>0.58760000000000001</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D21" s="2">
         <v>1.6574</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E21" s="2">
         <v>0.96009999999999995</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F21" s="2">
         <v>0.1152</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G21" s="2">
         <v>0</v>
       </c>
-      <c r="H19" s="2">
-        <v>2.9396</v>
-      </c>
-      <c r="I19" s="2">
+      <c r="H21" s="2">
+        <v>2.9306000000000001</v>
+      </c>
+      <c r="I21" s="2">
         <v>0.33939999999999998</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J21" s="2">
         <v>0</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K21" s="2">
         <v>1.7119</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L21" s="6">
         <v>0.317</v>
       </c>
-      <c r="M19" s="4">
+      <c r="M21" s="6">
         <v>0</v>
       </c>
-      <c r="N19" s="4">
+      <c r="N21" s="6">
         <v>0.73899999999999999</v>
       </c>
-      <c r="O19" s="2">
+      <c r="O21" s="2">
         <v>1.21</v>
       </c>
-      <c r="P19" s="2">
+      <c r="P21" s="2">
         <v>1</v>
       </c>
-      <c r="Q19" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="R19" s="2">
+      <c r="Q21" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="R21" s="2">
         <v>5.86</v>
       </c>
-      <c r="S19" s="2">
+      <c r="S21" s="2">
         <v>4</v>
       </c>
-      <c r="T19" s="2">
+      <c r="T21" s="2">
         <v>0.2102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="34">
-      <c r="A20" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="A21" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1.2482</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0.99209999999999998</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1.5705</v>
-      </c>
-      <c r="E22" s="1">
-        <v>5.8500000000000003E-2</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0.15390000000000001</v>
-      </c>
-      <c r="G22" s="1">
-        <v>6.2799999999999995E-2</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0.61270000000000002</v>
-      </c>
-      <c r="I22" s="1">
-        <v>0.39240000000000003</v>
-      </c>
-      <c r="J22" s="1">
-        <v>0.2505</v>
-      </c>
-      <c r="K22" s="1">
-        <v>0.78280000000000005</v>
+        <v>18</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.9869</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.58760000000000001</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1.6574</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.96009999999999995</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.1152</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2.9396</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.33939999999999998</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1.7119</v>
       </c>
       <c r="L22" s="4">
-        <v>0.79800000000000004</v>
+        <v>0.317</v>
       </c>
       <c r="M22" s="4">
-        <v>0.68100000000000005</v>
+        <v>0</v>
       </c>
       <c r="N22" s="4">
-        <v>0.873</v>
-      </c>
-      <c r="O22" s="1">
-        <v>2.23</v>
-      </c>
-      <c r="P22" s="1">
-        <v>1.77</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="R22" s="1">
-        <v>74.430000000000007</v>
-      </c>
-      <c r="S22" s="1">
-        <v>15</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="A23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1.1566000000000001</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0.95609999999999995</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1.3992</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0.1343</v>
-      </c>
-      <c r="F23" s="1">
-        <v>9.3299999999999994E-2</v>
-      </c>
-      <c r="G23" s="1">
-        <v>3.7100000000000001E-2</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0.51</v>
-      </c>
-      <c r="I23" s="1">
-        <v>0.30549999999999999</v>
-      </c>
-      <c r="J23" s="1">
-        <v>0.19270000000000001</v>
-      </c>
-      <c r="K23" s="1">
-        <v>0.71409999999999996</v>
-      </c>
-      <c r="L23" s="4">
-        <v>0.76900000000000002</v>
-      </c>
-      <c r="M23" s="4">
-        <v>0.627</v>
-      </c>
-      <c r="N23" s="4">
-        <v>0.85699999999999998</v>
-      </c>
-      <c r="O23" s="8">
-        <v>2.08</v>
-      </c>
-      <c r="P23" s="8">
-        <v>1.64</v>
-      </c>
-      <c r="Q23" s="8">
-        <v>2.64</v>
-      </c>
-      <c r="R23" s="8">
-        <v>64.84</v>
-      </c>
-      <c r="S23" s="8">
-        <v>15</v>
-      </c>
-      <c r="T23" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="31" customHeight="1">
-      <c r="A24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="O22" s="2">
+        <v>1.21</v>
+      </c>
+      <c r="P22" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="R22" s="2">
+        <v>5.86</v>
+      </c>
+      <c r="S22" s="2">
+        <v>4</v>
+      </c>
+      <c r="T22" s="2">
+        <v>0.2102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="34">
+      <c r="A23" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="1">
-        <v>1.9956</v>
+        <v>1.2482</v>
       </c>
       <c r="C25" s="1">
-        <v>1.4100999999999999</v>
+        <v>0.99209999999999998</v>
       </c>
       <c r="D25" s="1">
-        <v>2.8243</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>20</v>
+        <v>1.5705</v>
+      </c>
+      <c r="E25" s="1">
+        <v>5.8500000000000003E-2</v>
       </c>
       <c r="F25" s="1">
-        <v>0</v>
+        <v>0.15390000000000001</v>
       </c>
       <c r="G25" s="1">
-        <v>0</v>
+        <v>6.2799999999999995E-2</v>
       </c>
       <c r="H25" s="1">
-        <v>1.6114999999999999</v>
+        <v>0.61270000000000002</v>
       </c>
       <c r="I25" s="1">
-        <v>0</v>
+        <v>0.39240000000000003</v>
       </c>
       <c r="J25" s="1">
-        <v>0</v>
+        <v>0.2505</v>
       </c>
       <c r="K25" s="1">
-        <v>1.2694000000000001</v>
-      </c>
-      <c r="L25" s="9">
-        <v>0</v>
-      </c>
-      <c r="M25" s="9">
-        <v>0</v>
+        <v>0.78280000000000005</v>
+      </c>
+      <c r="L25" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="M25" s="4">
+        <v>0.68100000000000005</v>
       </c>
       <c r="N25" s="4">
-        <v>0.89600000000000002</v>
+        <v>0.873</v>
       </c>
       <c r="O25" s="1">
-        <v>1</v>
+        <v>2.23</v>
       </c>
       <c r="P25" s="1">
-        <v>1</v>
+        <v>1.77</v>
       </c>
       <c r="Q25" s="1">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="R25" s="1">
-        <v>0.44</v>
+        <v>74.430000000000007</v>
       </c>
       <c r="S25" s="1">
-        <v>2</v>
-      </c>
-      <c r="T25" s="1">
-        <v>0.80359999999999998</v>
+        <v>15</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -1741,62 +1746,219 @@
         <v>18</v>
       </c>
       <c r="B26" s="1">
+        <v>1.1566000000000001</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.95609999999999995</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1.3992</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.1343</v>
+      </c>
+      <c r="F26" s="1">
+        <v>9.3299999999999994E-2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.30549999999999999</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.19270000000000001</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0.71409999999999996</v>
+      </c>
+      <c r="L26" s="4">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="M26" s="4">
+        <v>0.627</v>
+      </c>
+      <c r="N26" s="4">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="O26" s="8">
+        <v>2.08</v>
+      </c>
+      <c r="P26" s="8">
+        <v>1.64</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>2.64</v>
+      </c>
+      <c r="R26" s="8">
+        <v>64.84</v>
+      </c>
+      <c r="S26" s="8">
+        <v>15</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="31" customHeight="1">
+      <c r="A27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1.9956</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1.4100999999999999</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2.8243</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1.6114999999999999</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <v>1.2694000000000001</v>
+      </c>
+      <c r="L28" s="9">
+        <v>0</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0</v>
+      </c>
+      <c r="N28" s="4">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="O28" s="1">
+        <v>1</v>
+      </c>
+      <c r="P28" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="R28" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="S28" s="1">
+        <v>2</v>
+      </c>
+      <c r="T28" s="1">
+        <v>0.80359999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="1">
         <v>1.9141999999999999</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C29" s="1">
         <v>1.3526</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D29" s="1">
         <v>2.7090000000000001</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E29" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F29" s="1">
         <v>0</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G29" s="1">
         <v>0</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H29" s="1">
         <v>2.0962999999999998</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I29" s="1">
         <v>0</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J29" s="1">
         <v>0</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K29" s="1">
         <v>1.4479</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L29" s="9">
         <v>0</v>
       </c>
-      <c r="M26" s="9">
+      <c r="M29" s="9">
         <v>0</v>
       </c>
-      <c r="N26" s="4">
+      <c r="N29" s="4">
         <v>0.89600000000000002</v>
       </c>
-      <c r="O26" s="1">
+      <c r="O29" s="1">
         <v>1</v>
       </c>
-      <c r="P26" s="1">
+      <c r="P29" s="1">
         <v>1</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="Q29" s="1">
         <v>3.1</v>
       </c>
-      <c r="R26" s="1">
+      <c r="R29" s="1">
         <v>0.62</v>
       </c>
-      <c r="S26" s="1">
+      <c r="S29" s="1">
         <v>2</v>
       </c>
-      <c r="T26" s="1">
+      <c r="T29" s="1">
         <v>0.73299999999999998</v>
       </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1806,10 +1968,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14342425-87E0-E64B-8C2B-7324AE590318}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1865,116 +2027,100 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="34">
+    <row r="3" spans="1:9" ht="29" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="17" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1">
-        <v>0.23185</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2.0400000000000001E-2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.25441000000000003</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.73839999999999995</v>
-      </c>
-      <c r="F4" s="1">
-        <v>4.0899999999999999E-2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.83599999999999997</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="17" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1">
-        <v>0.23616999999999999</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1.29E-2</v>
-      </c>
-      <c r="D5" s="1">
-        <v>-0.10277</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.88529999999999998</v>
-      </c>
-      <c r="F5" s="1">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.67869999999999997</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="34">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.23185</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.0400000000000001E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.25441000000000003</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.73839999999999995</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4.0899999999999999E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I7" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1">
-        <v>0.28289999999999998</v>
+        <v>0.23616999999999999</v>
       </c>
       <c r="C8" s="1">
-        <v>3.6299999999999999E-2</v>
+        <v>1.29E-2</v>
       </c>
       <c r="D8" s="1">
-        <v>0.82299999999999995</v>
+        <v>-0.10277</v>
       </c>
       <c r="E8" s="1">
-        <v>0.47889999999999999</v>
+        <v>0.88529999999999998</v>
       </c>
       <c r="F8" s="1">
-        <v>0.1111</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="G8" s="1">
-        <v>0.76139999999999997</v>
+        <v>0.67869999999999997</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>38</v>
@@ -1984,37 +2130,21 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.30230000000000001</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2.41E-2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.25600000000000001</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.81540000000000001</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.16669999999999999</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.61219999999999997</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0.5</v>
-      </c>
+      <c r="A9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2026,37 +2156,37 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="2" t="s">
-        <v>16</v>
+      <c r="A11" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B11" s="1">
-        <v>-4.1149999999999999E-2</v>
+        <v>0.28289999999999998</v>
       </c>
       <c r="C11" s="1">
-        <v>0.70399999999999996</v>
+        <v>3.6299999999999999E-2</v>
       </c>
       <c r="D11" s="1">
-        <v>0.40244000000000002</v>
+        <v>0.82299999999999995</v>
       </c>
       <c r="E11" s="1">
-        <v>0.55500000000000005</v>
+        <v>0.47889999999999999</v>
       </c>
       <c r="F11" s="1">
-        <v>0.15559999999999999</v>
+        <v>0.1111</v>
       </c>
       <c r="G11" s="1">
-        <v>0.60070000000000001</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0.25</v>
+        <v>0.76139999999999997</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="2" t="s">
-        <v>18</v>
+      <c r="A12" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B12" s="1">
         <v>0.30230000000000001</v>
@@ -2076,52 +2206,76 @@
       <c r="G12" s="1">
         <v>0.61219999999999997</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="2">
+      <c r="H12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="1">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-4.1149999999999999E-2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.40244000000000002</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.15559999999999999</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.60070000000000001</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0.19989999999999999</v>
-      </c>
-      <c r="C15" s="2">
-        <v>9.7900000000000001E-2</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.74619999999999997</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.49559999999999998</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0.1429</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0.51829999999999998</v>
+        <v>18</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.30230000000000001</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2.41E-2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.81540000000000001</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.61219999999999997</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>40</v>
@@ -2131,37 +2285,13 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0.22509999999999999</v>
-      </c>
-      <c r="C16" s="1">
-        <v>5.4100000000000002E-2</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0.10539999999999999</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0.91810000000000003</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0.20880000000000001</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0.33079999999999998</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0.5</v>
+      <c r="A16" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2176,28 +2306,28 @@
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1">
-        <v>-0.91290000000000004</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2.0019</v>
+      <c r="B18" s="2">
+        <v>0.19989999999999999</v>
+      </c>
+      <c r="C18" s="2">
+        <v>9.7900000000000001E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.74619999999999997</v>
       </c>
       <c r="E18" s="2">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0.48330000000000001</v>
+        <v>0.49559999999999998</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.1429</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.51829999999999998</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="2">
         <v>0.5</v>
       </c>
     </row>
@@ -2206,22 +2336,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>-0.91290000000000004</v>
+        <v>0.22509999999999999</v>
       </c>
       <c r="C19" s="1">
-        <v>0.18</v>
+        <v>5.4100000000000002E-2</v>
       </c>
       <c r="D19" s="1">
-        <v>2.0019</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.19500000000000001</v>
+        <v>0.10539999999999999</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.91810000000000003</v>
       </c>
       <c r="F19" s="1">
-        <v>0.4</v>
+        <v>0.20880000000000001</v>
       </c>
       <c r="G19" s="1">
-        <v>0.48330000000000001</v>
+        <v>0.33079999999999998</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>40</v>
@@ -2230,37 +2360,69 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="19" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>28</v>
-      </c>
+    <row r="20" spans="1:9">
+      <c r="A20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="5" t="s">
-        <v>29</v>
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>-0.91290000000000004</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2.0019</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.48330000000000001</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1">
-        <v>0.25685999999999998</v>
+        <v>-0.91290000000000004</v>
       </c>
       <c r="C22" s="1">
-        <v>2.1700000000000001E-2</v>
+        <v>0.18</v>
       </c>
       <c r="D22" s="1">
-        <v>-0.15264</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.86560000000000004</v>
+        <v>2.0019</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.19500000000000001</v>
       </c>
       <c r="F22" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G22" s="1">
-        <v>1</v>
+        <v>0.48330000000000001</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>40</v>
@@ -2269,38 +2431,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0.26683000000000001</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1.09E-2</v>
-      </c>
-      <c r="D23" s="1">
-        <v>-0.59362000000000004</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0.4743</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1">
-        <v>1</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="33" customHeight="1">
-      <c r="A24" s="3" t="s">
-        <v>30</v>
+    <row r="23" spans="1:9" ht="19" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2308,27 +2446,27 @@
         <v>16</v>
       </c>
       <c r="B25" s="1">
-        <v>0.41921999999999998</v>
+        <v>0.25685999999999998</v>
       </c>
       <c r="C25" s="1">
-        <v>8.0500000000000002E-2</v>
+        <v>2.1700000000000001E-2</v>
       </c>
       <c r="D25" s="1">
-        <v>0.96182999999999996</v>
+        <v>-0.15264</v>
       </c>
       <c r="E25" s="1">
-        <v>0.1138</v>
+        <v>0.86560000000000004</v>
       </c>
       <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
         <v>1</v>
-      </c>
-      <c r="G25" s="1">
-        <v>0.33329999999999999</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="1">
         <v>0.5</v>
       </c>
     </row>
@@ -2337,27 +2475,90 @@
         <v>18</v>
       </c>
       <c r="B26" s="1">
+        <v>0.26683000000000001</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1.09E-2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>-0.59362000000000004</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.4743</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="33" customHeight="1">
+      <c r="A27" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.41921999999999998</v>
+      </c>
+      <c r="C28" s="1">
+        <v>8.0500000000000002E-2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.96182999999999996</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.1138</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="1">
         <v>0.32079000000000002</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C29" s="1">
         <v>3.4599999999999999E-2</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D29" s="1">
         <v>1.16279</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E29" s="1">
         <v>3.1099999999999999E-2</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F29" s="1">
         <v>1</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G29" s="1">
         <v>0.33329999999999999</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I29" s="2">
         <v>0.25</v>
       </c>
     </row>

</xml_diff>